<commit_message>
finish version 1.0 of GS board
yay!
</commit_message>
<xml_diff>
--- a/GS module pin usage.xlsx
+++ b/GS module pin usage.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16260" windowHeight="20560" tabRatio="500"/>
+    <workbookView xWindow="16300" yWindow="0" windowWidth="16320" windowHeight="20560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="calculation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>RX1</t>
   </si>
@@ -75,9 +76,6 @@
     <t>THROT MODE ENGAGE</t>
   </si>
   <si>
-    <t>FLT-SD/ISO</t>
-  </si>
-  <si>
     <t>Hin1_ISO</t>
   </si>
   <si>
@@ -85,6 +83,90 @@
   </si>
   <si>
     <t>FLT_CLR1</t>
+  </si>
+  <si>
+    <t>END STOP UP</t>
+  </si>
+  <si>
+    <t>END STOP DN</t>
+  </si>
+  <si>
+    <t>mechanical switches / hall effect switches to detect completed shift</t>
+  </si>
+  <si>
+    <t>Need clutch switch</t>
+  </si>
+  <si>
+    <t>clutch engage before shift into neutral</t>
+  </si>
+  <si>
+    <t>FLT_CLR2</t>
+  </si>
+  <si>
+    <t>Hin2_ISO</t>
+  </si>
+  <si>
+    <t>Lin2_ISO</t>
+  </si>
+  <si>
+    <t>FLT-SD/ISO2</t>
+  </si>
+  <si>
+    <t>FLT-SD/ISO1</t>
+  </si>
+  <si>
+    <t>TEMP SENSOR</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Vin</t>
+  </si>
+  <si>
+    <t>Vout</t>
+  </si>
+  <si>
+    <t>TEMP1</t>
+  </si>
+  <si>
+    <t>TEMP2</t>
+  </si>
+  <si>
+    <t>CLUTCH SW</t>
+  </si>
+  <si>
+    <t>CONN</t>
+  </si>
+  <si>
+    <t>switch on wheel to shift up - SHIFT 3</t>
+  </si>
+  <si>
+    <t>switch on wheel to shift dn - SHIFT 2</t>
+  </si>
+  <si>
+    <t>NOTE 2</t>
+  </si>
+  <si>
+    <t>ENDSTOPS 3</t>
+  </si>
+  <si>
+    <t>ENDSTOPS 2</t>
+  </si>
+  <si>
+    <t>MODE_SEL 4</t>
+  </si>
+  <si>
+    <t>MODE_SEL 3</t>
+  </si>
+  <si>
+    <t>MODE_SEL 2</t>
+  </si>
+  <si>
+    <t>MODE_SEL 1</t>
   </si>
 </sst>
 </file>
@@ -116,7 +198,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +217,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -145,7 +239,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -159,25 +253,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -507,20 +607,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -530,8 +630,14 @@
       <c r="C1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>0</v>
       </c>
@@ -541,8 +647,9 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -552,8 +659,9 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>2</v>
       </c>
@@ -561,10 +669,11 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>30</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>3</v>
       </c>
@@ -572,10 +681,11 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>4</v>
       </c>
@@ -583,10 +693,11 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>19</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>5</v>
       </c>
@@ -594,15 +705,20 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>7</v>
       </c>
@@ -610,10 +726,11 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>8</v>
       </c>
@@ -621,10 +738,11 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>27</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>9</v>
       </c>
@@ -632,10 +750,11 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>28</v>
+      </c>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>10</v>
       </c>
@@ -643,22 +762,23 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>26</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>13</v>
       </c>
@@ -668,44 +788,81 @@
       <c r="C15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -715,8 +872,12 @@
       <c r="C22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22" s="4"/>
+      <c r="E22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -726,8 +887,12 @@
       <c r="C23" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23" s="4"/>
+      <c r="E23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -737,8 +902,12 @@
       <c r="C24" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24" s="4"/>
+      <c r="E24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -747,6 +916,18 @@
       </c>
       <c r="C25" t="s">
         <v>16</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -758,4 +939,65 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <f>B3/(B2+B3)*B4</f>
+        <v>3.2142857142857144</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Versions of the board which went to the fab house
Updating BOMS for component ordering
</commit_message>
<xml_diff>
--- a/GS module pin usage.xlsx
+++ b/GS module pin usage.xlsx
@@ -4,13 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16300" yWindow="0" windowWidth="16320" windowHeight="20560" tabRatio="500"/>
+    <workbookView xWindow="2080" yWindow="3260" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="pins" sheetId="1" r:id="rId1"/>
     <sheet name="calculation" sheetId="2" r:id="rId2"/>
+    <sheet name="dimension" sheetId="3" r:id="rId3"/>
+    <sheet name="BOm" sheetId="4" r:id="rId4"/>
+    <sheet name="Pivot" sheetId="6" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="GS_mod_bom" localSheetId="3">BOm!$A$1:$F$50</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="14" r:id="rId6"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,8 +28,25 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="GS_mod_bom.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="FRANKSSSD:Users:frank:Documents:university:2015:FYP repos:electrical:GS_mod_bom.txt" delimited="0">
+      <textFields count="6">
+        <textField type="text"/>
+        <textField position="12"/>
+        <textField position="36"/>
+        <textField position="59"/>
+        <textField position="86"/>
+        <textField position="108"/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="195">
   <si>
     <t>RX1</t>
   </si>
@@ -167,6 +193,444 @@
   </si>
   <si>
     <t>MODE_SEL 1</t>
+  </si>
+  <si>
+    <t>SHIFT LEVER</t>
+  </si>
+  <si>
+    <t>SHIFT LEVER POT</t>
+  </si>
+  <si>
+    <t>Partlist</t>
+  </si>
+  <si>
+    <t>Exported fro</t>
+  </si>
+  <si>
+    <t>m GS_module.brd at 1/09/</t>
+  </si>
+  <si>
+    <t>2015 9:18</t>
+  </si>
+  <si>
+    <t>EAGLE Versio</t>
+  </si>
+  <si>
+    <t>n 7.3.0 Copyright (c) 19</t>
+  </si>
+  <si>
+    <t>88-2015 CadSoft</t>
+  </si>
+  <si>
+    <t>Assembly var</t>
+  </si>
+  <si>
+    <t>iant:</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>Position (inch)</t>
+  </si>
+  <si>
+    <t>Orientation</t>
+  </si>
+  <si>
+    <t>10VZENER</t>
+  </si>
+  <si>
+    <t>DO214BA</t>
+  </si>
+  <si>
+    <t>diode</t>
+  </si>
+  <si>
+    <t>(0.3 0.85)</t>
+  </si>
+  <si>
+    <t>MR90</t>
+  </si>
+  <si>
+    <t>BAT_CONN</t>
+  </si>
+  <si>
+    <t>W237-132</t>
+  </si>
+  <si>
+    <t>con-wago-508</t>
+  </si>
+  <si>
+    <t>(0.2 1.425)</t>
+  </si>
+  <si>
+    <t>R270</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>C1206</t>
+  </si>
+  <si>
+    <t>resistor</t>
+  </si>
+  <si>
+    <t>(1.125 0.7)</t>
+  </si>
+  <si>
+    <t>MR180</t>
+  </si>
+  <si>
+    <t>CLUTCH_SW</t>
+  </si>
+  <si>
+    <t>(2.45 1.25)</t>
+  </si>
+  <si>
+    <t>R90</t>
+  </si>
+  <si>
+    <t>ENDSTOPS</t>
+  </si>
+  <si>
+    <t>W237-133</t>
+  </si>
+  <si>
+    <t>(0.85 3)</t>
+  </si>
+  <si>
+    <t>R180</t>
+  </si>
+  <si>
+    <t>GSENDSTOP</t>
+  </si>
+  <si>
+    <t>(2.45 0.7)</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>P0-11</t>
+  </si>
+  <si>
+    <t>1X12_LOCK</t>
+  </si>
+  <si>
+    <t>SparkFun-Connectors</t>
+  </si>
+  <si>
+    <t>(1.7 0.8)</t>
+  </si>
+  <si>
+    <t>JP2</t>
+  </si>
+  <si>
+    <t>P12-23</t>
+  </si>
+  <si>
+    <t>(0.8 1)</t>
+  </si>
+  <si>
+    <t>JP3</t>
+  </si>
+  <si>
+    <t>SER</t>
+  </si>
+  <si>
+    <t>MOLEX-1X3_LOCK</t>
+  </si>
+  <si>
+    <t>(1.65 0.3)</t>
+  </si>
+  <si>
+    <t>MODE_SEL</t>
+  </si>
+  <si>
+    <t>W237-5P</t>
+  </si>
+  <si>
+    <t>(0.175 2.15)</t>
+  </si>
+  <si>
+    <t>MOTECSIGNAL</t>
+  </si>
+  <si>
+    <t>(2.45 2.85)</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>MOSFET-PCHANNELFQP27P06</t>
+  </si>
+  <si>
+    <t>TO220V</t>
+  </si>
+  <si>
+    <t>SparkFun-DiscreteSemi</t>
+  </si>
+  <si>
+    <t>(0.225 1.075)</t>
+  </si>
+  <si>
+    <t>R1206</t>
+  </si>
+  <si>
+    <t>rcl</t>
+  </si>
+  <si>
+    <t>(1.825 0.825)</t>
+  </si>
+  <si>
+    <t>(1.8 1.975)</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>(1.825 1.05)</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>(1.8 2.2)</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>(0.35 1.3)</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>(1.9 2.85)</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>(1.5 2.85)</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>4.7k</t>
+  </si>
+  <si>
+    <t>(2.05 2.7)</t>
+  </si>
+  <si>
+    <t>R0</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>(1.4 2.2)</t>
+  </si>
+  <si>
+    <t>MR0</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>(2.25 2.35)</t>
+  </si>
+  <si>
+    <t>MR270</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>(2.25 2.075)</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>(0.65 2.7)</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>(0.85 2.7)</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>(0.45 2.35)</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>(0.45 2.15)</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>(0.45 1.95)</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>(0.45 1.75)</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>(2.25 1.4)</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>LOGIC POWER</t>
+  </si>
+  <si>
+    <t>SWITCH-SPDT_KIT</t>
+  </si>
+  <si>
+    <t>SparkFun-Electromechanical</t>
+  </si>
+  <si>
+    <t>(0.6 0.3)</t>
+  </si>
+  <si>
+    <t>SHIFT</t>
+  </si>
+  <si>
+    <t>(2.45 2.15)</t>
+  </si>
+  <si>
+    <t>SOLDVR1</t>
+  </si>
+  <si>
+    <t>1X10_LOCK</t>
+  </si>
+  <si>
+    <t>(1.95 1.2)</t>
+  </si>
+  <si>
+    <t>SOLDVR2</t>
+  </si>
+  <si>
+    <t>(1.95 2.35)</t>
+  </si>
+  <si>
+    <t>U$1</t>
+  </si>
+  <si>
+    <t>TEENSY31DEV</t>
+  </si>
+  <si>
+    <t>TEENSY31PAC</t>
+  </si>
+  <si>
+    <t>custom</t>
+  </si>
+  <si>
+    <t>(1.3 1.35)</t>
+  </si>
+  <si>
+    <t>U$3</t>
+  </si>
+  <si>
+    <t>NPN_TRAN</t>
+  </si>
+  <si>
+    <t>SOT23-3</t>
+  </si>
+  <si>
+    <t>(1.65 2.7)</t>
+  </si>
+  <si>
+    <t>U$4</t>
+  </si>
+  <si>
+    <t>PNP_TRAN</t>
+  </si>
+  <si>
+    <t>(1.65 2.95)</t>
+  </si>
+  <si>
+    <t>U$5</t>
+  </si>
+  <si>
+    <t>TRACOTMR2WIN</t>
+  </si>
+  <si>
+    <t>TRACOPOWERDC-DCTRM2WIN</t>
+  </si>
+  <si>
+    <t>(0.15 0.475)</t>
+  </si>
+  <si>
+    <t>U$6</t>
+  </si>
+  <si>
+    <t>LNBTVS</t>
+  </si>
+  <si>
+    <t>JEDECDO-214AB</t>
+  </si>
+  <si>
+    <t>(0.55 0.75)</t>
+  </si>
+  <si>
+    <t>U$17</t>
+  </si>
+  <si>
+    <t>OPTOISOLATOR-2SOIC8</t>
+  </si>
+  <si>
+    <t>SO08-2</t>
+  </si>
+  <si>
+    <t>(1.6 2.4)</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of Part</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -198,7 +662,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,6 +693,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -239,7 +709,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -255,15 +725,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -271,6 +747,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -278,11 +755,588 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Francis Conroy" refreshedDate="42248.414818634257" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="41">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A9:F50" sheet="BOm"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="Part" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Value" numFmtId="0">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="15" maxValue="270" count="19">
+        <m/>
+        <s v="0.1uF"/>
+        <s v="P0-11"/>
+        <s v="P12-23"/>
+        <s v="SER"/>
+        <s v="MOSFET-PCHANNELFQP27P06"/>
+        <n v="27"/>
+        <n v="15"/>
+        <s v="1k"/>
+        <n v="270"/>
+        <s v="10k"/>
+        <s v="4.7k"/>
+        <s v="LOGIC POWER"/>
+        <s v="TEENSY31DEV"/>
+        <s v="NPN_TRAN"/>
+        <s v="PNP_TRAN"/>
+        <s v="TRACOTMR2WIN"/>
+        <s v="LNBTVS"/>
+        <s v="OPTOISOLATOR-2SOIC8"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Package" numFmtId="0">
+      <sharedItems containsBlank="1" count="17">
+        <m/>
+        <s v="DO214BA"/>
+        <s v="W237-132"/>
+        <s v="C1206"/>
+        <s v="W237-133"/>
+        <s v="1X12_LOCK"/>
+        <s v="MOLEX-1X3_LOCK"/>
+        <s v="W237-5P"/>
+        <s v="TO220V"/>
+        <s v="R1206"/>
+        <s v="SWITCH-SPDT_KIT"/>
+        <s v="1X10_LOCK"/>
+        <s v="TEENSY31PAC"/>
+        <s v="SOT23-3"/>
+        <s v="TRACOPOWERDC-DCTRM2WIN"/>
+        <s v="JEDECDO-214AB"/>
+        <s v="SO08-2"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Library" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Position (inch)" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Orientation" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="41">
+  <r>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="10VZENER"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="diode"/>
+    <s v="(0.3 0.85)"/>
+    <s v="MR90"/>
+  </r>
+  <r>
+    <s v="BAT_CONN"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="con-wago-508"/>
+    <s v="(0.2 1.425)"/>
+    <s v="R270"/>
+  </r>
+  <r>
+    <s v="C1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <s v="resistor"/>
+    <s v="(1.125 0.7)"/>
+    <s v="MR180"/>
+  </r>
+  <r>
+    <s v="CLUTCH_SW"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="con-wago-508"/>
+    <s v="(2.45 1.25)"/>
+    <s v="R90"/>
+  </r>
+  <r>
+    <s v="ENDSTOPS"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="con-wago-508"/>
+    <s v="(0.85 3)"/>
+    <s v="R180"/>
+  </r>
+  <r>
+    <s v="GSENDSTOP"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="con-wago-508"/>
+    <s v="(2.45 0.7)"/>
+    <s v="R90"/>
+  </r>
+  <r>
+    <s v="JP1"/>
+    <x v="2"/>
+    <x v="5"/>
+    <s v="SparkFun-Connectors"/>
+    <s v="(1.7 0.8)"/>
+    <s v="R90"/>
+  </r>
+  <r>
+    <s v="JP2"/>
+    <x v="3"/>
+    <x v="5"/>
+    <s v="SparkFun-Connectors"/>
+    <s v="(0.8 1)"/>
+    <s v="R90"/>
+  </r>
+  <r>
+    <s v="JP3"/>
+    <x v="4"/>
+    <x v="6"/>
+    <s v="SparkFun-Connectors"/>
+    <s v="(1.65 0.3)"/>
+    <s v="R180"/>
+  </r>
+  <r>
+    <s v="MODE_SEL"/>
+    <x v="0"/>
+    <x v="7"/>
+    <s v="con-wago-508"/>
+    <s v="(0.175 2.15)"/>
+    <s v="R90"/>
+  </r>
+  <r>
+    <s v="MOTECSIGNAL"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="con-wago-508"/>
+    <s v="(2.45 2.85)"/>
+    <s v="R270"/>
+  </r>
+  <r>
+    <s v="Q2"/>
+    <x v="5"/>
+    <x v="8"/>
+    <s v="SparkFun-DiscreteSemi"/>
+    <s v="(0.225 1.075)"/>
+    <s v="R180"/>
+  </r>
+  <r>
+    <s v="R1"/>
+    <x v="6"/>
+    <x v="9"/>
+    <s v="rcl"/>
+    <s v="(1.825 0.825)"/>
+    <s v="MR90"/>
+  </r>
+  <r>
+    <s v="R2"/>
+    <x v="6"/>
+    <x v="9"/>
+    <s v="rcl"/>
+    <s v="(1.8 1.975)"/>
+    <s v="MR90"/>
+  </r>
+  <r>
+    <s v="R3"/>
+    <x v="7"/>
+    <x v="9"/>
+    <s v="rcl"/>
+    <s v="(1.825 1.05)"/>
+    <s v="MR90"/>
+  </r>
+  <r>
+    <s v="R4"/>
+    <x v="7"/>
+    <x v="9"/>
+    <s v="rcl"/>
+    <s v="(1.8 2.2)"/>
+    <s v="MR90"/>
+  </r>
+  <r>
+    <s v="R5"/>
+    <x v="8"/>
+    <x v="9"/>
+    <s v="rcl"/>
+    <s v="(0.35 1.3)"/>
+    <s v="MR90"/>
+  </r>
+  <r>
+    <s v="R6"/>
+    <x v="9"/>
+    <x v="9"/>
+    <s v="resistor"/>
+    <s v="(1.9 2.85)"/>
+    <s v="MR90"/>
+  </r>
+  <r>
+    <s v="R7"/>
+    <x v="10"/>
+    <x v="9"/>
+    <s v="resistor"/>
+    <s v="(1.5 2.85)"/>
+    <s v="R270"/>
+  </r>
+  <r>
+    <s v="R8"/>
+    <x v="11"/>
+    <x v="9"/>
+    <s v="resistor"/>
+    <s v="(2.05 2.7)"/>
+    <s v="R0"/>
+  </r>
+  <r>
+    <s v="R9"/>
+    <x v="8"/>
+    <x v="9"/>
+    <s v="resistor"/>
+    <s v="(1.4 2.2)"/>
+    <s v="MR0"/>
+  </r>
+  <r>
+    <s v="R10"/>
+    <x v="10"/>
+    <x v="9"/>
+    <s v="rcl"/>
+    <s v="(2.25 2.35)"/>
+    <s v="MR270"/>
+  </r>
+  <r>
+    <s v="R11"/>
+    <x v="10"/>
+    <x v="9"/>
+    <s v="rcl"/>
+    <s v="(2.25 2.075)"/>
+    <s v="MR270"/>
+  </r>
+  <r>
+    <s v="R12"/>
+    <x v="10"/>
+    <x v="9"/>
+    <s v="rcl"/>
+    <s v="(0.65 2.7)"/>
+    <s v="MR270"/>
+  </r>
+  <r>
+    <s v="R13"/>
+    <x v="10"/>
+    <x v="9"/>
+    <s v="rcl"/>
+    <s v="(0.85 2.7)"/>
+    <s v="MR270"/>
+  </r>
+  <r>
+    <s v="R14"/>
+    <x v="10"/>
+    <x v="9"/>
+    <s v="rcl"/>
+    <s v="(0.45 2.35)"/>
+    <s v="MR180"/>
+  </r>
+  <r>
+    <s v="R15"/>
+    <x v="10"/>
+    <x v="9"/>
+    <s v="rcl"/>
+    <s v="(0.45 2.15)"/>
+    <s v="MR180"/>
+  </r>
+  <r>
+    <s v="R16"/>
+    <x v="10"/>
+    <x v="9"/>
+    <s v="rcl"/>
+    <s v="(0.45 1.95)"/>
+    <s v="MR180"/>
+  </r>
+  <r>
+    <s v="R17"/>
+    <x v="10"/>
+    <x v="9"/>
+    <s v="rcl"/>
+    <s v="(0.45 1.75)"/>
+    <s v="MR180"/>
+  </r>
+  <r>
+    <s v="R18"/>
+    <x v="10"/>
+    <x v="9"/>
+    <s v="rcl"/>
+    <s v="(2.25 1.4)"/>
+    <s v="MR90"/>
+  </r>
+  <r>
+    <s v="S1"/>
+    <x v="12"/>
+    <x v="10"/>
+    <s v="SparkFun-Electromechanical"/>
+    <s v="(0.6 0.3)"/>
+    <s v="R0"/>
+  </r>
+  <r>
+    <s v="SHIFT"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="con-wago-508"/>
+    <s v="(2.45 2.15)"/>
+    <s v="R90"/>
+  </r>
+  <r>
+    <s v="SOLDVR1"/>
+    <x v="0"/>
+    <x v="11"/>
+    <s v="SparkFun-Connectors"/>
+    <s v="(1.95 1.2)"/>
+    <s v="R270"/>
+  </r>
+  <r>
+    <s v="SOLDVR2"/>
+    <x v="0"/>
+    <x v="11"/>
+    <s v="SparkFun-Connectors"/>
+    <s v="(1.95 2.35)"/>
+    <s v="R270"/>
+  </r>
+  <r>
+    <s v="U$1"/>
+    <x v="13"/>
+    <x v="12"/>
+    <s v="custom"/>
+    <s v="(1.3 1.35)"/>
+    <s v="R90"/>
+  </r>
+  <r>
+    <s v="U$3"/>
+    <x v="14"/>
+    <x v="13"/>
+    <s v="custom"/>
+    <s v="(1.65 2.7)"/>
+    <s v="R0"/>
+  </r>
+  <r>
+    <s v="U$4"/>
+    <x v="15"/>
+    <x v="13"/>
+    <s v="custom"/>
+    <s v="(1.65 2.95)"/>
+    <s v="R180"/>
+  </r>
+  <r>
+    <s v="U$5"/>
+    <x v="16"/>
+    <x v="14"/>
+    <s v="custom"/>
+    <s v="(0.15 0.475)"/>
+    <s v="R270"/>
+  </r>
+  <r>
+    <s v="U$6"/>
+    <x v="17"/>
+    <x v="15"/>
+    <s v="custom"/>
+    <s v="(0.55 0.75)"/>
+    <s v="R270"/>
+  </r>
+  <r>
+    <s v="U$17"/>
+    <x v="18"/>
+    <x v="16"/>
+    <s v="SparkFun-DiscreteSemi"/>
+    <s v="(1.6 2.4)"/>
+    <s v="R180"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A3:C29" firstHeaderRow="2" firstDataRow="2" firstDataCol="2"/>
+  <pivotFields count="6">
+    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <items count="19">
+        <item x="7"/>
+        <item x="6"/>
+        <item x="9"/>
+        <item x="1"/>
+        <item x="10"/>
+        <item x="8"/>
+        <item x="11"/>
+        <item x="17"/>
+        <item x="12"/>
+        <item x="5"/>
+        <item x="14"/>
+        <item x="18"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="15"/>
+        <item x="4"/>
+        <item x="13"/>
+        <item x="16"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
+      <items count="17">
+        <item x="11"/>
+        <item x="5"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="15"/>
+        <item x="6"/>
+        <item x="9"/>
+        <item x="16"/>
+        <item x="13"/>
+        <item x="10"/>
+        <item x="12"/>
+        <item x="8"/>
+        <item x="14"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="0"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0"/>
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0"/>
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="25">
+    <i>
+      <x/>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="8"/>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="9"/>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="10"/>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="11"/>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="12"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="13"/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="14"/>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="15"/>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="16"/>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="17"/>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="18"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Part" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GS_mod_bom" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -609,8 +1663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -770,13 +1824,25 @@
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
@@ -795,24 +1861,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="4"/>
+        <v>50</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1">
@@ -1000,4 +2058,1245 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1">
+        <v>2.65</v>
+      </c>
+      <c r="B1">
+        <f>A1*25.4</f>
+        <v>67.309999999999988</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>3.2</v>
+      </c>
+      <c r="B2">
+        <f>25.4*A2</f>
+        <v>81.28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3">
+        <f t="shared" ref="B3:B6" si="0">25.4*A3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>101.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>3.2</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>81.28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:F50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" t="s">
+        <v>105</v>
+      </c>
+      <c r="F20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" t="s">
+        <v>114</v>
+      </c>
+      <c r="E25" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" t="s">
+        <v>123</v>
+      </c>
+      <c r="F27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28">
+        <v>270</v>
+      </c>
+      <c r="C28" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" t="s">
+        <v>125</v>
+      </c>
+      <c r="F28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" t="s">
+        <v>128</v>
+      </c>
+      <c r="F29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" t="s">
+        <v>130</v>
+      </c>
+      <c r="C30" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" t="s">
+        <v>131</v>
+      </c>
+      <c r="F30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" t="s">
+        <v>134</v>
+      </c>
+      <c r="F31" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" t="s">
+        <v>114</v>
+      </c>
+      <c r="E32" t="s">
+        <v>137</v>
+      </c>
+      <c r="F32" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" t="s">
+        <v>114</v>
+      </c>
+      <c r="E33" t="s">
+        <v>140</v>
+      </c>
+      <c r="F33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" t="s">
+        <v>114</v>
+      </c>
+      <c r="E34" t="s">
+        <v>142</v>
+      </c>
+      <c r="F34" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B35" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" t="s">
+        <v>144</v>
+      </c>
+      <c r="F35" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B36" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" t="s">
+        <v>114</v>
+      </c>
+      <c r="E36" t="s">
+        <v>146</v>
+      </c>
+      <c r="F36" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" t="s">
+        <v>114</v>
+      </c>
+      <c r="E37" t="s">
+        <v>148</v>
+      </c>
+      <c r="F37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B38" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" t="s">
+        <v>114</v>
+      </c>
+      <c r="E38" t="s">
+        <v>150</v>
+      </c>
+      <c r="F38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B39" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" t="s">
+        <v>114</v>
+      </c>
+      <c r="E39" t="s">
+        <v>152</v>
+      </c>
+      <c r="F39" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B40" t="s">
+        <v>127</v>
+      </c>
+      <c r="C40" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" t="s">
+        <v>114</v>
+      </c>
+      <c r="E40" t="s">
+        <v>154</v>
+      </c>
+      <c r="F40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B41" t="s">
+        <v>156</v>
+      </c>
+      <c r="C41" t="s">
+        <v>157</v>
+      </c>
+      <c r="D41" t="s">
+        <v>158</v>
+      </c>
+      <c r="E41" t="s">
+        <v>159</v>
+      </c>
+      <c r="F41" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42" t="s">
+        <v>161</v>
+      </c>
+      <c r="F42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C43" t="s">
+        <v>163</v>
+      </c>
+      <c r="D43" t="s">
+        <v>94</v>
+      </c>
+      <c r="E43" t="s">
+        <v>164</v>
+      </c>
+      <c r="F43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C44" t="s">
+        <v>163</v>
+      </c>
+      <c r="D44" t="s">
+        <v>94</v>
+      </c>
+      <c r="E44" t="s">
+        <v>166</v>
+      </c>
+      <c r="F44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B45" t="s">
+        <v>168</v>
+      </c>
+      <c r="C45" t="s">
+        <v>169</v>
+      </c>
+      <c r="D45" t="s">
+        <v>170</v>
+      </c>
+      <c r="E45" t="s">
+        <v>171</v>
+      </c>
+      <c r="F45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B46" t="s">
+        <v>173</v>
+      </c>
+      <c r="C46" t="s">
+        <v>174</v>
+      </c>
+      <c r="D46" t="s">
+        <v>170</v>
+      </c>
+      <c r="E46" t="s">
+        <v>175</v>
+      </c>
+      <c r="F46" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B47" t="s">
+        <v>177</v>
+      </c>
+      <c r="C47" t="s">
+        <v>174</v>
+      </c>
+      <c r="D47" t="s">
+        <v>170</v>
+      </c>
+      <c r="E47" t="s">
+        <v>178</v>
+      </c>
+      <c r="F47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B48" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" t="s">
+        <v>181</v>
+      </c>
+      <c r="D48" t="s">
+        <v>170</v>
+      </c>
+      <c r="E48" t="s">
+        <v>182</v>
+      </c>
+      <c r="F48" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B49" t="s">
+        <v>184</v>
+      </c>
+      <c r="C49" t="s">
+        <v>185</v>
+      </c>
+      <c r="D49" t="s">
+        <v>170</v>
+      </c>
+      <c r="E49" t="s">
+        <v>186</v>
+      </c>
+      <c r="F49" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B50" t="s">
+        <v>188</v>
+      </c>
+      <c r="C50" t="s">
+        <v>189</v>
+      </c>
+      <c r="D50" t="s">
+        <v>111</v>
+      </c>
+      <c r="E50" t="s">
+        <v>190</v>
+      </c>
+      <c r="F50" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:C29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" customWidth="1"/>
+    <col min="13" max="13" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="31" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="41" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="6.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3">
+      <c r="A3" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>270</v>
+      </c>
+      <c r="B7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" t="s">
+        <v>185</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B16" t="s">
+        <v>189</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" t="s">
+        <v>174</v>
+      </c>
+      <c r="C19" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" t="s">
+        <v>169</v>
+      </c>
+      <c r="C21" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>180</v>
+      </c>
+      <c r="B22" t="s">
+        <v>181</v>
+      </c>
+      <c r="C22" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>191</v>
+      </c>
+      <c r="B23" t="s">
+        <v>163</v>
+      </c>
+      <c r="C23" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="B27" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="B28" t="s">
+        <v>191</v>
+      </c>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>192</v>
+      </c>
+      <c r="C29" s="8">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>